<commit_message>
Proposal and diagram1 ready -DF
</commit_message>
<xml_diff>
--- a/Agent.xlsx
+++ b/Agent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\repos\intuitive_agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6741C96F-876C-4681-B3D8-1AB73B0F424C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3A7CB0-5205-4C43-B29E-AF8669E494D3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="7005" xr2:uid="{3A381773-1E35-425C-A91C-4E8EA81612AD}"/>
   </bookViews>
@@ -25,67 +25,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">Context Pipes - </t>
-  </si>
-  <si>
-    <t>ANN 1</t>
-  </si>
-  <si>
-    <t>ANN 2</t>
-  </si>
-  <si>
-    <t>ANN 3</t>
-  </si>
-  <si>
-    <t>Pipe 1</t>
-  </si>
-  <si>
-    <t>Pipe 2</t>
-  </si>
-  <si>
-    <t>Pipe 3</t>
-  </si>
-  <si>
-    <t>Pipe n</t>
-  </si>
-  <si>
-    <t>Agent focuses on some combination of inputs</t>
-  </si>
-  <si>
-    <t>ANN out represents classification of that input</t>
-  </si>
-  <si>
-    <t>Sensory input</t>
-  </si>
-  <si>
-    <t>Feedback Input 1</t>
-  </si>
-  <si>
-    <t>Feedback Input 2</t>
-  </si>
-  <si>
-    <t>Feedback Input 3</t>
-  </si>
-  <si>
-    <t>Feedback Input n</t>
-  </si>
-  <si>
-    <t>ANN</t>
-  </si>
-  <si>
-    <t>Selected Pipes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each pipe is weighted according to </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+  <si>
+    <t>Feedback Inputs</t>
+  </si>
+  <si>
+    <t>ANN_n</t>
+  </si>
+  <si>
+    <t>ANN_0</t>
+  </si>
+  <si>
+    <t>ANN_1</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Sensory Inputs</t>
+  </si>
+  <si>
+    <t>Pipe_1_IN</t>
+  </si>
+  <si>
+    <t>Pipe_2_IN</t>
+  </si>
+  <si>
+    <t>Pipe_n_IN</t>
+  </si>
+  <si>
+    <t>Intuitive Layer</t>
+  </si>
+  <si>
+    <t>Attentive Layer</t>
+  </si>
+  <si>
+    <t>Conceptual Layer</t>
+  </si>
+  <si>
+    <t>(Represents pre-learned abstract concepts)</t>
+  </si>
+  <si>
+    <t>(pre-trained)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Represents intuitive abstract connections) </t>
+  </si>
+  <si>
+    <t>(Represents current awareness)</t>
+  </si>
+  <si>
+    <t>P1_WEIGHTED_OUT</t>
+  </si>
+  <si>
+    <t>P2_WEIGHTED_OUT</t>
+  </si>
+  <si>
+    <t>Pn_WEIGHTED_OUT</t>
+  </si>
+  <si>
+    <t>Evolving Weight Function</t>
+  </si>
+  <si>
+    <t>(Repr. links between conceptual-layer concepts)</t>
+  </si>
+  <si>
+    <t>A_ANN</t>
+  </si>
+  <si>
+    <t>Fitness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +108,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,12 +159,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -158,19 +220,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -231,35 +280,203 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,185 +791,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B031D8-174E-485C-B176-ECA6C65A7406}">
-  <dimension ref="B4:K24"/>
+  <dimension ref="B4:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.73046875" customWidth="1"/>
-    <col min="2" max="2" width="16.3984375" customWidth="1"/>
+    <col min="1" max="1" width="1.9296875" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="3.46484375" customWidth="1"/>
     <col min="4" max="4" width="15.46484375" customWidth="1"/>
-    <col min="8" max="8" width="17.59765625" customWidth="1"/>
-    <col min="9" max="9" width="23.1328125" customWidth="1"/>
+    <col min="5" max="5" width="4.53125" customWidth="1"/>
+    <col min="6" max="6" width="4.265625" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" customWidth="1"/>
+    <col min="8" max="8" width="12.19921875" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="5.265625" customWidth="1"/>
+    <col min="11" max="11" width="5.06640625" customWidth="1"/>
+    <col min="14" max="14" width="9.59765625" customWidth="1"/>
+    <col min="15" max="15" width="9.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="H4" t="s">
+    <row r="4" spans="2:14" s="32" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4"/>
+      <c r="H4" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4"/>
+      <c r="M4" s="33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="26"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+    </row>
+    <row r="9" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+    </row>
+    <row r="10" spans="2:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="12" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="14"/>
+      <c r="L12" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="35"/>
+      <c r="N12" s="40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C13" s="7"/>
+      <c r="D13" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="41"/>
+    </row>
+    <row r="14" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="16"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="41"/>
+    </row>
+    <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G15" s="13"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="17"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="41"/>
+    </row>
+    <row r="16" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="15"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="41"/>
+    </row>
+    <row r="17" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C17" s="7"/>
+      <c r="D17" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="41"/>
+    </row>
+    <row r="18" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="16"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="41"/>
+    </row>
+    <row r="19" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G19" s="13"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="17"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="41"/>
+    </row>
+    <row r="20" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="15"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="41"/>
+    </row>
+    <row r="21" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C21" s="7"/>
+      <c r="D21" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="41"/>
+    </row>
+    <row r="22" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="19"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="16"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="41"/>
+    </row>
+    <row r="23" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G23" s="13"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="17"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="41"/>
+    </row>
+    <row r="24" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="15"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="41"/>
+    </row>
+    <row r="25" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C25" s="7"/>
+      <c r="D25" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="9" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C10" s="17"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="11"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="H12" s="3"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C14" s="17"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="11"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="H16" s="3"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="15" t="s">
+      <c r="H25" s="9"/>
+      <c r="I25" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="41"/>
+    </row>
+    <row r="26" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C18" s="17"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="11"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="H20" s="3"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C22" s="17"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="11"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="H24" s="4"/>
-      <c r="I24" s="14"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="16"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="41"/>
+    </row>
+    <row r="27" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G27" s="13"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="17"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="42"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="H30" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H22:H23"/>
+  <mergeCells count="11">
+    <mergeCell ref="L12:M27"/>
+    <mergeCell ref="N12:N27"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I17:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>